<commit_message>
Added Uber minicase data
</commit_message>
<xml_diff>
--- a/Uber_Minicase/Uber_Dispatching_Data.xlsx
+++ b/Uber_Minicase/Uber_Dispatching_Data.xlsx
@@ -8,181 +8,182 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Dropbox\Academic\INSEAD\Teaching\2021\ARM_FBL_March\Cases\Uber Minicase\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B785BAA-3871-4148-BCF4-CA55C6B89FE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C6ABA0-DAF0-41FA-92ED-6614665A1F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38890" yWindow="1020" windowWidth="34850" windowHeight="19360" tabRatio="850" xr2:uid="{33A83AC2-AE54-4FD9-B8E6-EA6E160DC162}"/>
+    <workbookView xWindow="41900" yWindow="1400" windowWidth="34850" windowHeight="19360" tabRatio="850" activeTab="1" xr2:uid="{33A83AC2-AE54-4FD9-B8E6-EA6E160DC162}"/>
   </bookViews>
   <sheets>
     <sheet name="Drivers" sheetId="45" r:id="rId1"/>
-    <sheet name="Riders" sheetId="46" r:id="rId2"/>
-    <sheet name="Q6_data" sheetId="42" r:id="rId3"/>
-    <sheet name="Q7_data" sheetId="43" r:id="rId4"/>
+    <sheet name="Josephines_Match" sheetId="47" r:id="rId2"/>
+    <sheet name="Riders" sheetId="46" r:id="rId3"/>
+    <sheet name="Q6_data" sheetId="42" r:id="rId4"/>
+    <sheet name="Q7_data" sheetId="43" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">Q6_data!#REF!,Q6_data!#REF!</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Q6_data!#REF!,Q6_data!#REF!</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_ibd" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ibd" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs0" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs4" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs5" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs6" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_lhs6" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs7" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lhs8" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_lin" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_lva" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_lhs0" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_lhs5" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_lhs6" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs7" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lhs8" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_lin" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_lva" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">4</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">6</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_ofx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_ofx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Drivers!#REF!</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">Riders!#REF!</definedName>
-    <definedName name="solver_piv" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Riders!#REF!</definedName>
+    <definedName name="solver_piv" localSheetId="4" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.0001</definedName>
-    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
-    <definedName name="solver_pro" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pro" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_red" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_rel0" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_rel1" localSheetId="3" hidden="1">4</definedName>
-    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_red" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rel0" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">5</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="2" hidden="1">5</definedName>
-    <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="3" hidden="1">5</definedName>
+    <definedName name="solver_rel4" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rel6" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel6" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel7" localSheetId="3" hidden="1">4</definedName>
-    <definedName name="solver_rel8" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_reo" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rep" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rhs0" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">binary</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Integer</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_rhs4" localSheetId="2" hidden="1">binary</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_rhs5" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_rhs5" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
-    <definedName name="solver_rhs6" localSheetId="2" hidden="1">Q6_data!#REF!</definedName>
-    <definedName name="solver_rhs6" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rhs7" localSheetId="3" hidden="1">[1]!Integer</definedName>
-    <definedName name="solver_rhs8" localSheetId="3" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_rel5" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="4" hidden="1">4</definedName>
+    <definedName name="solver_rel8" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_reo" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rep" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rhs0" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">binary</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">Integer</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">binary</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_rhs5" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">Q6_data!#REF!</definedName>
+    <definedName name="solver_rhs6" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rhs7" localSheetId="4" hidden="1">[1]!Integer</definedName>
+    <definedName name="solver_rhs8" localSheetId="4" hidden="1">Q7_data!#REF!</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
-    <definedName name="solver_std" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_std" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">30</definedName>
-    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" concurrentCalc="0"/>
   <extLst>
@@ -202,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>A</t>
   </si>
@@ -311,7 +312,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -319,12 +320,166 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -354,6 +509,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514ACDE3-D9CB-4AB7-A1B6-4188291F3DF7}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -831,6 +1006,218 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D70E93-6AF4-409C-ACD1-901E493F1619}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="15">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16">
+        <v>4</v>
+      </c>
+      <c r="F1" s="16">
+        <v>5</v>
+      </c>
+      <c r="G1" s="16">
+        <v>6</v>
+      </c>
+      <c r="H1" s="16">
+        <v>7</v>
+      </c>
+      <c r="I1" s="16">
+        <v>8</v>
+      </c>
+      <c r="J1" s="16">
+        <v>9</v>
+      </c>
+      <c r="K1" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20">
+        <v>1</v>
+      </c>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="24"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="24"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB826A5C-6B05-45D5-8600-0053CA1D0D2B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1042,7 +1429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1D8078-753D-4875-A9D2-4BF7CDDFAEDA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -1133,7 +1520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE8124D-14F3-46DB-83C6-E21D13EA9132}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>

</xml_diff>